<commit_message>
did stuff, mostly housekeeping
</commit_message>
<xml_diff>
--- a/docs/mp3 slicing.xlsx
+++ b/docs/mp3 slicing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edge9\source\repos\Arduino Projects\RetroPhone\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{486C40A3-8D85-4E96-9595-9C2B1F56A53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36E8D69-9033-4B96-AF22-1C2C71B20954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11790" yWindow="-20340" windowWidth="16935" windowHeight="19920" xr2:uid="{E7F5CC72-E50D-4F6F-899D-2913C47FFF53}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="27340" windowHeight="17620" xr2:uid="{E7F5CC72-E50D-4F6F-899D-2913C47FFF53}"/>
   </bookViews>
   <sheets>
     <sheet name="anna-1DSS-default-vocab.mp3" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Hz</t>
   </si>
@@ -135,8 +135,71 @@
     </r>
   </si>
   <si>
+    <t>please note</t>
+  </si>
+  <si>
+    <t>this is a recording</t>
+  </si>
+  <si>
+    <t>has been changed</t>
+  </si>
+  <si>
+    <t>the number you have dialed</t>
+  </si>
+  <si>
+    <t>is not in service</t>
+  </si>
+  <si>
+    <t>please check the number and dial again</t>
+  </si>
+  <si>
+    <t>the number dialed</t>
+  </si>
+  <si>
+    <t>the new number is</t>
+  </si>
+  <si>
+    <t>enter function</t>
+  </si>
+  <si>
+    <t>please enter</t>
+  </si>
+  <si>
+    <t>area code</t>
+  </si>
+  <si>
+    <t>new number</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>not available</t>
+  </si>
+  <si>
+    <t>enter service code</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>re-enter</t>
+  </si>
+  <si>
+    <t>thank you</t>
+  </si>
+  <si>
+    <t>or dial directory assistance</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Offset
+      <t xml:space="preserve">Adjust
 </t>
     </r>
     <r>
@@ -151,67 +214,57 @@
     </r>
   </si>
   <si>
-    <t>please note</t>
-  </si>
-  <si>
-    <t>this is a recording</t>
-  </si>
-  <si>
-    <t>has been changed</t>
-  </si>
-  <si>
-    <t>the number you have dialed</t>
-  </si>
-  <si>
-    <t>is not in service</t>
-  </si>
-  <si>
-    <t>please check the number and dial again</t>
-  </si>
-  <si>
-    <t>the number dialed</t>
-  </si>
-  <si>
-    <t>the new number is</t>
-  </si>
-  <si>
-    <t>enter function</t>
-  </si>
-  <si>
-    <t>please enter</t>
-  </si>
-  <si>
-    <t>area code</t>
-  </si>
-  <si>
-    <t>new number</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>not available</t>
-  </si>
-  <si>
-    <t>enter service code</t>
-  </si>
-  <si>
-    <t>deleted</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>re-enter</t>
-  </si>
-  <si>
-    <t>thank you</t>
-  </si>
-  <si>
-    <t>or dial directory assistance</t>
+    <r>
+      <t xml:space="preserve">Offset-calc
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bytes)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Offset-real
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bytes)</t>
+    </r>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>last sample</t>
+  </si>
+  <si>
+    <t>examine ramp sample</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>step size</t>
+  </si>
+  <si>
+    <t>examined step value</t>
+  </si>
+  <si>
+    <t>examined sample value</t>
   </si>
 </sst>
 </file>
@@ -590,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA54231D-B4DE-4F9B-943D-81A0A6B7D927}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,12 +657,15 @@
     <col min="5" max="6" width="6.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7265625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.08984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
       <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
@@ -620,16 +676,22 @@
         <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -654,14 +716,21 @@
         <v>4670.0869893292675</v>
       </c>
       <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <f>H2+I2</f>
+        <v>4670.0869893292675</v>
+      </c>
+      <c r="K2" s="5">
         <f>$B$5*G2</f>
         <v>23769.899999999998</v>
       </c>
-      <c r="J2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -687,14 +756,21 @@
         <v>8943.6005518292677</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I33" si="1">$B$5*G3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J33" si="1">H3+I3</f>
+        <v>8943.6005518292677</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K33" si="2">$B$5*G3</f>
         <v>18786.600000000002</v>
       </c>
-      <c r="J3" s="7">
+      <c r="L3" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -719,14 +795,21 @@
         <v>12519.561243902439</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="1"/>
+        <v>12519.561243902439</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" si="2"/>
         <v>18566.100000000002</v>
       </c>
-      <c r="J4" s="7">
+      <c r="L4" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -751,14 +834,21 @@
         <v>16087.504086890243</v>
       </c>
       <c r="I5" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="1"/>
+        <v>16087.504086890243</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" si="2"/>
         <v>19580.399999999998</v>
       </c>
-      <c r="J5" s="7">
+      <c r="L5" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -783,14 +873,27 @@
         <v>19767.696817073171</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="1"/>
+        <v>19767.696817073171</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="2"/>
         <v>17684.099999999991</v>
       </c>
-      <c r="J6" s="7">
+      <c r="L6" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>1024</v>
+      </c>
+      <c r="O6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -816,14 +919,27 @@
         <v>23014.92569664634</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="1"/>
+        <v>23014.92569664634</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="2"/>
         <v>27650.700000000012</v>
       </c>
-      <c r="J7" s="7">
+      <c r="L7" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>-50</v>
+      </c>
+      <c r="O7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E8" s="3">
         <v>3.2309999999999999</v>
       </c>
@@ -839,14 +955,32 @@
         <v>28290.670394817069</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="1"/>
+        <v>28290.670394817069</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="2"/>
         <v>23681.699999999997</v>
       </c>
-      <c r="J8" s="7">
+      <c r="L8" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <f>127-N7</f>
+        <v>177</v>
+      </c>
+      <c r="O8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <f>B2/B7/1000</f>
+        <v>8.106923018292683</v>
+      </c>
       <c r="E9" s="3">
         <v>3.7869999999999999</v>
       </c>
@@ -862,14 +996,28 @@
         <v>32748.594486280486</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="1"/>
+        <v>32748.594486280486</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="2"/>
         <v>18610.199999999986</v>
       </c>
-      <c r="J9" s="7">
+      <c r="L9" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <f>N8/N6</f>
+        <v>0.1728515625</v>
+      </c>
+      <c r="O9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E10" s="3">
         <v>4.2140000000000004</v>
       </c>
@@ -885,14 +1033,27 @@
         <v>36172.216045731708</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="1"/>
+        <v>36172.216045731708</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="2"/>
         <v>18213.299999999974</v>
       </c>
-      <c r="J10" s="7">
+      <c r="L10" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>128</v>
+      </c>
+      <c r="O10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E11" s="3">
         <v>4.625</v>
       </c>
@@ -908,14 +1069,28 @@
         <v>39467.552019817071</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="1"/>
+        <v>39467.552019817071</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="2"/>
         <v>25048.799999999985</v>
       </c>
-      <c r="J11" s="7">
+      <c r="L11" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <f>N10*N9</f>
+        <v>22.125</v>
+      </c>
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E12" s="3">
         <v>5.1950000000000003</v>
       </c>
@@ -931,14 +1106,28 @@
         <v>44037.725998475609</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="1"/>
+        <v>44037.725998475609</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="2"/>
         <v>23814</v>
       </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L12" s="7">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f>N11+N7</f>
+        <v>-27.875</v>
+      </c>
+      <c r="O12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E13" s="3">
         <v>5.7380000000000004</v>
       </c>
@@ -954,14 +1143,21 @@
         <v>48391.418051829271</v>
       </c>
       <c r="I13" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="1"/>
+        <v>48391.418051829271</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="2"/>
         <v>32810.399999999987</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L13" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E14" s="3">
         <v>6.484</v>
       </c>
@@ -977,14 +1173,21 @@
         <v>54372.73346951219</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="1"/>
+        <v>54372.73346951219</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="2"/>
         <v>48333.600000000006</v>
       </c>
-      <c r="J14" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L14" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E15" s="3">
         <v>7.5730000000000004</v>
       </c>
@@ -1000,14 +1203,21 @@
         <v>63104.171123475608</v>
       </c>
       <c r="I15" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="1"/>
+        <v>63104.171123475608</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="2"/>
         <v>52082.099999999962</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L15" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E16" s="3">
         <v>8.7530000000000001</v>
       </c>
@@ -1023,14 +1233,21 @@
         <v>72565.233044207314</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="1"/>
+        <v>72565.233044207314</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="2"/>
         <v>68002.2</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L16" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E17" s="3">
         <v>10.295</v>
       </c>
@@ -1046,14 +1263,21 @@
         <v>84928.756333841462</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="1"/>
+        <v>84928.756333841462</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="2"/>
         <v>57065.400000000023</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L17" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E18" s="3">
         <v>11.593</v>
       </c>
@@ -1068,15 +1292,19 @@
         <f>($B$4/$B$7*E18) + $B$3</f>
         <v>95335.924446646342</v>
       </c>
-      <c r="I18" s="5">
-        <f t="shared" si="1"/>
+      <c r="J18" s="5">
+        <f t="shared" si="1"/>
+        <v>95335.924446646342</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="2"/>
         <v>98343.000000000015</v>
       </c>
-      <c r="J18" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L18" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E19" s="3">
         <v>13.819000000000001</v>
       </c>
@@ -1091,15 +1319,19 @@
         <f>($B$4/$B$7*E19) + $B$3</f>
         <v>113183.65651067073</v>
       </c>
-      <c r="I19" s="5">
-        <f t="shared" si="1"/>
+      <c r="J19" s="5">
+        <f t="shared" si="1"/>
+        <v>113183.65651067073</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="2"/>
         <v>48333.599999999926</v>
       </c>
-      <c r="J19" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L19" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E20" s="3">
         <v>14.914999999999999</v>
       </c>
@@ -1114,15 +1346,19 @@
         <f>($B$4/$B$7*E20) + $B$3</f>
         <v>121971.2191082317</v>
       </c>
-      <c r="I20" s="5">
-        <f t="shared" si="1"/>
+      <c r="J20" s="5">
+        <f t="shared" si="1"/>
+        <v>121971.2191082317</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="2"/>
         <v>57771.000000000102</v>
       </c>
-      <c r="J20" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L20" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E21" s="3">
         <v>16.225000000000001</v>
       </c>
@@ -1137,15 +1373,19 @@
         <f>($B$4/$B$7*E21) + $B$3</f>
         <v>132474.60141006098</v>
       </c>
-      <c r="I21" s="5">
-        <f t="shared" si="1"/>
+      <c r="J21" s="5">
+        <f t="shared" si="1"/>
+        <v>132474.60141006098</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="2"/>
         <v>31840.199999999903</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L21" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E22" s="3">
         <v>16.946999999999999</v>
       </c>
@@ -1160,15 +1400,19 @@
         <f>($B$4/$B$7*E22) + $B$3</f>
         <v>138263.48844969511</v>
       </c>
-      <c r="I22" s="5">
-        <f t="shared" si="1"/>
+      <c r="J22" s="5">
+        <f t="shared" si="1"/>
+        <v>138263.48844969511</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="2"/>
         <v>29547.000000000076</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L22" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E23" s="3">
         <v>17.617000000000001</v>
       </c>
@@ -1183,15 +1427,19 @@
         <f>($B$4/$B$7*E23) + $B$3</f>
         <v>143635.44733689024</v>
       </c>
-      <c r="I23" s="5">
-        <f t="shared" si="1"/>
+      <c r="J23" s="5">
+        <f t="shared" si="1"/>
+        <v>143635.44733689024</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="2"/>
         <v>33912.899999999929</v>
       </c>
-      <c r="J23" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L23" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E24" s="3">
         <v>18.385999999999999</v>
       </c>
@@ -1206,15 +1454,19 @@
         <f>($B$4/$B$7*E24) + $B$3</f>
         <v>149801.17328353657</v>
       </c>
-      <c r="I24" s="5">
-        <f t="shared" si="1"/>
+      <c r="J24" s="5">
+        <f t="shared" si="1"/>
+        <v>149801.17328353657</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="2"/>
         <v>27782.999999999956</v>
       </c>
-      <c r="J24" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L24" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E25" s="3">
         <v>19.015999999999998</v>
       </c>
@@ -1229,15 +1481,19 @@
         <f>($B$4/$B$7*E25) + $B$3</f>
         <v>154852.41820731704</v>
       </c>
-      <c r="I25" s="5">
-        <f t="shared" si="1"/>
+      <c r="J25" s="5">
+        <f t="shared" si="1"/>
+        <v>154852.41820731704</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="2"/>
         <v>27562.5</v>
       </c>
-      <c r="J25" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L25" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E26" s="3">
         <v>19.640999999999998</v>
       </c>
@@ -1252,15 +1508,19 @@
         <f>($B$4/$B$7*E26) + $B$3</f>
         <v>159863.57388567072</v>
       </c>
-      <c r="I26" s="5">
-        <f t="shared" si="1"/>
+      <c r="J26" s="5">
+        <f t="shared" si="1"/>
+        <v>159863.57388567072</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="2"/>
         <v>32413.500000000131</v>
       </c>
-      <c r="J26" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L26" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E27" s="3">
         <v>20.376000000000001</v>
       </c>
@@ -1275,15 +1535,19 @@
         <f>($B$4/$B$7*E27) + $B$3</f>
         <v>165756.69296341462</v>
       </c>
-      <c r="I27" s="5">
-        <f t="shared" si="1"/>
+      <c r="J27" s="5">
+        <f t="shared" si="1"/>
+        <v>165756.69296341462</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="2"/>
         <v>57418.199999999983</v>
       </c>
-      <c r="J27" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E28" s="3">
         <v>21.678000000000001</v>
       </c>
@@ -1298,15 +1562,19 @@
         <f>($B$4/$B$7*E28) + $B$3</f>
         <v>176195.93247256096</v>
       </c>
-      <c r="I28" s="5">
-        <f t="shared" si="1"/>
+      <c r="J28" s="5">
+        <f t="shared" si="1"/>
+        <v>176195.93247256096</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="2"/>
         <v>21344.399999999921</v>
       </c>
-      <c r="J28" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L28" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E29" s="3">
         <v>22.161999999999999</v>
       </c>
@@ -1321,15 +1589,19 @@
         <f>($B$4/$B$7*E29) + $B$3</f>
         <v>180076.57142987804</v>
       </c>
-      <c r="I29" s="5">
-        <f t="shared" si="1"/>
+      <c r="J29" s="5">
+        <f t="shared" si="1"/>
+        <v>180076.57142987804</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="2"/>
         <v>28488.600000000035</v>
       </c>
-      <c r="J29" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L29" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E30" s="3">
         <v>22.808</v>
       </c>
@@ -1344,15 +1616,19 @@
         <f>($B$4/$B$7*E30) + $B$3</f>
         <v>185256.10193902437</v>
       </c>
-      <c r="I30" s="5">
-        <f t="shared" si="1"/>
+      <c r="J30" s="5">
+        <f t="shared" si="1"/>
+        <v>185256.10193902437</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="2"/>
         <v>17992.800000000054</v>
       </c>
-      <c r="J30" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L30" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E31" s="3">
         <v>23.216000000000001</v>
       </c>
@@ -1367,15 +1643,19 @@
         <f>($B$4/$B$7*E31) + $B$3</f>
         <v>188527.38436585365</v>
       </c>
-      <c r="I31" s="5">
-        <f t="shared" si="1"/>
+      <c r="J31" s="5">
+        <f t="shared" si="1"/>
+        <v>188527.38436585365</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="2"/>
         <v>25754.399999999983</v>
       </c>
-      <c r="J31" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L31" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E32" s="3">
         <v>23.8</v>
       </c>
@@ -1390,15 +1670,19 @@
         <f>($B$4/$B$7*E32) + $B$3</f>
         <v>193209.80823170731</v>
       </c>
-      <c r="I32" s="5">
-        <f t="shared" si="1"/>
+      <c r="J32" s="5">
+        <f t="shared" si="1"/>
+        <v>193209.80823170731</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="2"/>
         <v>20550.599999999889</v>
       </c>
-      <c r="J32" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="L32" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.35">
       <c r="E33" s="3">
         <v>24.265999999999998</v>
       </c>
@@ -1413,12 +1697,16 @@
         <f>($B$4/$B$7*E33) + $B$3</f>
         <v>196946.12590548777</v>
       </c>
-      <c r="I33" s="5">
-        <f t="shared" si="1"/>
+      <c r="J33" s="5">
+        <f t="shared" si="1"/>
+        <v>196946.12590548777</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="2"/>
         <v>75499.200000000143</v>
       </c>
-      <c r="J33" s="7" t="s">
-        <v>36</v>
+      <c r="L33" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to slices constant and added 1s before error playback sequence
</commit_message>
<xml_diff>
--- a/docs/mp3 slicing.xlsx
+++ b/docs/mp3 slicing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edge9\source\repos\Arduino Projects\RetroPhone\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36E8D69-9033-4B96-AF22-1C2C71B20954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2524B0D9-3A43-44B7-A8AD-FB601FE5E7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="27340" windowHeight="17620" xr2:uid="{E7F5CC72-E50D-4F6F-899D-2913C47FFF53}"/>
+    <workbookView xWindow="19995" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{E7F5CC72-E50D-4F6F-899D-2913C47FFF53}"/>
   </bookViews>
   <sheets>
     <sheet name="anna-1DSS-default-vocab.mp3" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -315,10 +315,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -646,7 +646,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,7 +712,7 @@
         <v>0.53899999999999992</v>
       </c>
       <c r="H2" s="5">
-        <f>($B$4/$B$7*E2) + $B$3</f>
+        <f t="shared" ref="H2:H33" si="0">($B$4/$B$7*E2) + $B$3</f>
         <v>4670.0869893292675</v>
       </c>
       <c r="I2" s="5">
@@ -748,22 +748,22 @@
         <v>1.244</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G33" si="0">F3-E3</f>
+        <f t="shared" ref="G3:G33" si="1">F3-E3</f>
         <v>0.42600000000000005</v>
       </c>
       <c r="H3" s="5">
-        <f>($B$4/$B$7*E3) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>8943.6005518292677</v>
       </c>
       <c r="I3" s="5">
         <v>0</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J33" si="1">H3+I3</f>
+        <f t="shared" ref="J3:J33" si="2">H3+I3</f>
         <v>8943.6005518292677</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K33" si="2">$B$5*G3</f>
+        <f t="shared" ref="K3:K33" si="3">$B$5*G3</f>
         <v>18786.600000000002</v>
       </c>
       <c r="L3" s="7">
@@ -787,22 +787,22 @@
         <v>1.6850000000000001</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42100000000000004</v>
       </c>
       <c r="H4" s="5">
-        <f>($B$4/$B$7*E4) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>12519.561243902439</v>
       </c>
       <c r="I4" s="5">
         <v>0</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12519.561243902439</v>
       </c>
       <c r="K4" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18566.100000000002</v>
       </c>
       <c r="L4" s="7">
@@ -826,22 +826,22 @@
         <v>2.153</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.44399999999999995</v>
       </c>
       <c r="H5" s="5">
-        <f>($B$4/$B$7*E5) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>16087.504086890243</v>
       </c>
       <c r="I5" s="5">
         <v>0</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16087.504086890243</v>
       </c>
       <c r="K5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19580.399999999998</v>
       </c>
       <c r="L5" s="7">
@@ -865,22 +865,22 @@
         <v>2.569</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4009999999999998</v>
       </c>
       <c r="H6" s="5">
-        <f>($B$4/$B$7*E6) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>19767.696817073171</v>
       </c>
       <c r="I6" s="5">
         <v>0</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19767.696817073171</v>
       </c>
       <c r="K6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17684.099999999991</v>
       </c>
       <c r="L6" s="7">
@@ -911,22 +911,22 @@
         <v>3.2</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.62700000000000022</v>
       </c>
       <c r="H7" s="5">
-        <f>($B$4/$B$7*E7) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>23014.92569664634</v>
       </c>
       <c r="I7" s="5">
         <v>0</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23014.92569664634</v>
       </c>
       <c r="K7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27650.700000000012</v>
       </c>
       <c r="L7" s="7">
@@ -947,22 +947,22 @@
         <v>3.7679999999999998</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.53699999999999992</v>
       </c>
       <c r="H8" s="5">
-        <f>($B$4/$B$7*E8) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>28290.670394817069</v>
       </c>
       <c r="I8" s="5">
         <v>0</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28290.670394817069</v>
       </c>
       <c r="K8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23681.699999999997</v>
       </c>
       <c r="L8" s="7">
@@ -977,10 +977,6 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9">
-        <f>B2/B7/1000</f>
-        <v>8.106923018292683</v>
-      </c>
       <c r="E9" s="3">
         <v>3.7869999999999999</v>
       </c>
@@ -988,22 +984,22 @@
         <v>4.2089999999999996</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.42199999999999971</v>
       </c>
       <c r="H9" s="5">
-        <f>($B$4/$B$7*E9) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>32748.594486280486</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32748.594486280486</v>
       </c>
       <c r="K9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18610.199999999986</v>
       </c>
       <c r="L9" s="7">
@@ -1025,22 +1021,22 @@
         <v>4.6269999999999998</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.41299999999999937</v>
       </c>
       <c r="H10" s="5">
-        <f>($B$4/$B$7*E10) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>36172.216045731708</v>
       </c>
       <c r="I10" s="5">
         <v>0</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36172.216045731708</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18213.299999999974</v>
       </c>
       <c r="L10" s="7">
@@ -1061,22 +1057,22 @@
         <v>5.1929999999999996</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.56799999999999962</v>
       </c>
       <c r="H11" s="5">
-        <f>($B$4/$B$7*E11) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>39467.552019817071</v>
       </c>
       <c r="I11" s="5">
         <v>0</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39467.552019817071</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25048.799999999985</v>
       </c>
       <c r="L11" s="7">
@@ -1098,22 +1094,22 @@
         <v>5.7350000000000003</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.54</v>
       </c>
       <c r="H12" s="5">
-        <f>($B$4/$B$7*E12) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>44037.725998475609</v>
       </c>
       <c r="I12" s="5">
         <v>0</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44037.725998475609</v>
       </c>
       <c r="K12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23814</v>
       </c>
       <c r="L12" s="7">
@@ -1135,22 +1131,22 @@
         <v>6.4820000000000002</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.74399999999999977</v>
       </c>
       <c r="H13" s="5">
-        <f>($B$4/$B$7*E13) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>48391.418051829271</v>
       </c>
       <c r="I13" s="5">
         <v>0</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48391.418051829271</v>
       </c>
       <c r="K13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32810.399999999987</v>
       </c>
       <c r="L13" s="7" t="s">
@@ -1165,22 +1161,22 @@
         <v>7.58</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0960000000000001</v>
       </c>
       <c r="H14" s="5">
-        <f>($B$4/$B$7*E14) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>54372.73346951219</v>
       </c>
       <c r="I14" s="5">
         <v>0</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54372.73346951219</v>
       </c>
       <c r="K14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48333.600000000006</v>
       </c>
       <c r="L14" s="7" t="s">
@@ -1195,22 +1191,22 @@
         <v>8.7539999999999996</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1809999999999992</v>
       </c>
       <c r="H15" s="5">
-        <f>($B$4/$B$7*E15) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>63104.171123475608</v>
       </c>
       <c r="I15" s="5">
         <v>0</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63104.171123475608</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52082.099999999962</v>
       </c>
       <c r="L15" s="7" t="s">
@@ -1225,22 +1221,22 @@
         <v>10.295</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5419999999999998</v>
       </c>
       <c r="H16" s="5">
-        <f>($B$4/$B$7*E16) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>72565.233044207314</v>
       </c>
       <c r="I16" s="5">
         <v>0</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72565.233044207314</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>68002.2</v>
       </c>
       <c r="L16" s="7" t="s">
@@ -1255,22 +1251,22 @@
         <v>11.589</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2940000000000005</v>
       </c>
       <c r="H17" s="5">
-        <f>($B$4/$B$7*E17) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>84928.756333841462</v>
       </c>
       <c r="I17" s="5">
         <v>0</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84928.756333841462</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57065.400000000023</v>
       </c>
       <c r="L17" s="7" t="s">
@@ -1285,19 +1281,19 @@
         <v>13.823</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2300000000000004</v>
       </c>
       <c r="H18" s="5">
-        <f>($B$4/$B$7*E18) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>95335.924446646342</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95335.924446646342</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>98343.000000000015</v>
       </c>
       <c r="L18" s="7" t="s">
@@ -1312,19 +1308,19 @@
         <v>14.914999999999999</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0959999999999983</v>
       </c>
       <c r="H19" s="5">
-        <f>($B$4/$B$7*E19) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>113183.65651067073</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113183.65651067073</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48333.599999999926</v>
       </c>
       <c r="L19" s="7" t="s">
@@ -1339,19 +1335,19 @@
         <v>16.225000000000001</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3100000000000023</v>
       </c>
       <c r="H20" s="5">
-        <f>($B$4/$B$7*E20) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>121971.2191082317</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121971.2191082317</v>
       </c>
       <c r="K20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57771.000000000102</v>
       </c>
       <c r="L20" s="7" t="s">
@@ -1366,19 +1362,19 @@
         <v>16.946999999999999</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.72199999999999775</v>
       </c>
       <c r="H21" s="5">
-        <f>($B$4/$B$7*E21) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>132474.60141006098</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>132474.60141006098</v>
       </c>
       <c r="K21" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31840.199999999903</v>
       </c>
       <c r="L21" s="7" t="s">
@@ -1393,19 +1389,19 @@
         <v>17.617000000000001</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.67000000000000171</v>
       </c>
       <c r="H22" s="5">
-        <f>($B$4/$B$7*E22) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>138263.48844969511</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>138263.48844969511</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29547.000000000076</v>
       </c>
       <c r="L22" s="7" t="s">
@@ -1420,19 +1416,19 @@
         <v>18.385999999999999</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.76899999999999835</v>
       </c>
       <c r="H23" s="5">
-        <f>($B$4/$B$7*E23) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>143635.44733689024</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>143635.44733689024</v>
       </c>
       <c r="K23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33912.899999999929</v>
       </c>
       <c r="L23" s="7" t="s">
@@ -1447,19 +1443,19 @@
         <v>19.015999999999998</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.62999999999999901</v>
       </c>
       <c r="H24" s="5">
-        <f>($B$4/$B$7*E24) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>149801.17328353657</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>149801.17328353657</v>
       </c>
       <c r="K24" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27782.999999999956</v>
       </c>
       <c r="L24" s="7" t="s">
@@ -1474,19 +1470,19 @@
         <v>19.640999999999998</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
       <c r="H25" s="5">
-        <f>($B$4/$B$7*E25) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>154852.41820731704</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>154852.41820731704</v>
       </c>
       <c r="K25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27562.5</v>
       </c>
       <c r="L25" s="7" t="s">
@@ -1501,19 +1497,19 @@
         <v>20.376000000000001</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.73500000000000298</v>
       </c>
       <c r="H26" s="5">
-        <f>($B$4/$B$7*E26) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>159863.57388567072</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>159863.57388567072</v>
       </c>
       <c r="K26" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32413.500000000131</v>
       </c>
       <c r="L26" s="7" t="s">
@@ -1528,19 +1524,19 @@
         <v>21.678000000000001</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3019999999999996</v>
       </c>
       <c r="H27" s="5">
-        <f>($B$4/$B$7*E27) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>165756.69296341462</v>
       </c>
       <c r="J27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>165756.69296341462</v>
       </c>
       <c r="K27" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57418.199999999983</v>
       </c>
       <c r="L27" s="7" t="s">
@@ -1555,19 +1551,19 @@
         <v>22.161999999999999</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.48399999999999821</v>
       </c>
       <c r="H28" s="5">
-        <f>($B$4/$B$7*E28) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>176195.93247256096</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>176195.93247256096</v>
       </c>
       <c r="K28" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21344.399999999921</v>
       </c>
       <c r="L28" s="7" t="s">
@@ -1582,19 +1578,19 @@
         <v>22.808</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6460000000000008</v>
       </c>
       <c r="H29" s="5">
-        <f>($B$4/$B$7*E29) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>180076.57142987804</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>180076.57142987804</v>
       </c>
       <c r="K29" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28488.600000000035</v>
       </c>
       <c r="L29" s="7" t="s">
@@ -1609,19 +1605,19 @@
         <v>23.216000000000001</v>
       </c>
       <c r="G30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40800000000000125</v>
       </c>
       <c r="H30" s="5">
-        <f>($B$4/$B$7*E30) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>185256.10193902437</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>185256.10193902437</v>
       </c>
       <c r="K30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17992.800000000054</v>
       </c>
       <c r="L30" s="7" t="s">
@@ -1636,19 +1632,19 @@
         <v>23.8</v>
       </c>
       <c r="G31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.58399999999999963</v>
       </c>
       <c r="H31" s="5">
-        <f>($B$4/$B$7*E31) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>188527.38436585365</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>188527.38436585365</v>
       </c>
       <c r="K31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25754.399999999983</v>
       </c>
       <c r="L31" s="7" t="s">
@@ -1663,19 +1659,19 @@
         <v>24.265999999999998</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.46599999999999753</v>
       </c>
       <c r="H32" s="5">
-        <f>($B$4/$B$7*E32) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>193209.80823170731</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>193209.80823170731</v>
       </c>
       <c r="K32" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20550.599999999889</v>
       </c>
       <c r="L32" s="7" t="s">
@@ -1690,19 +1686,19 @@
         <v>25.978000000000002</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7120000000000033</v>
       </c>
       <c r="H33" s="5">
-        <f>($B$4/$B$7*E33) + $B$3</f>
+        <f t="shared" si="0"/>
         <v>196946.12590548777</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>196946.12590548777</v>
       </c>
       <c r="K33" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75499.200000000143</v>
       </c>
       <c r="L33" s="7" t="s">

</xml_diff>